<commit_message>
added comments to code and started adding detailed instructions to part 2 of the notebook
</commit_message>
<xml_diff>
--- a/ABC Subsidiary.xlsx
+++ b/ABC Subsidiary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reid.nelson\Trial Balance Import - Quickbook Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D67C8D4-9A4E-4CF9-ABE6-7CC399D2EF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2D970A-F6C4-47DB-8EC8-499B4CD8FC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickBooks Desktop Export Tips" sheetId="2" r:id="rId1"/>
@@ -24,45 +24,25 @@
     <definedName name="QB_COLUMN_57200" localSheetId="1" hidden="1">Sheet1!$C$5</definedName>
     <definedName name="QB_COLUMN_58210" localSheetId="1" hidden="1">Sheet1!$E$5</definedName>
     <definedName name="QB_COMPANY_0" localSheetId="1" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="QB_DATA_0" localSheetId="1" hidden="1">Sheet1!$6:$6,Sheet1!$7:$7,Sheet1!$8:$8,Sheet1!$9:$9,Sheet1!$10:$10,Sheet1!$11:$11,Sheet1!$12:$12,Sheet1!$13:$13,Sheet1!$14:$14,Sheet1!$15:$15,Sheet1!$16:$16,Sheet1!$17:$17,Sheet1!$18:$18,Sheet1!$19:$19,Sheet1!$20:$20,Sheet1!$21:$21</definedName>
-    <definedName name="QB_DATA_1" localSheetId="1" hidden="1">Sheet1!$22:$22,Sheet1!$23:$23,Sheet1!$24:$24,Sheet1!$25:$25,Sheet1!$26:$26,Sheet1!$27:$27,Sheet1!$28:$28,Sheet1!$29:$29,Sheet1!$30:$30,Sheet1!$31:$31,Sheet1!$32:$32,Sheet1!$33:$33,Sheet1!$34:$34</definedName>
+    <definedName name="QB_DATA_0" localSheetId="1" hidden="1">Sheet1!$6:$6,Sheet1!$7:$7,Sheet1!$8:$8,Sheet1!$9:$9,Sheet1!$10:$10,Sheet1!$11:$11,Sheet1!$12:$12,Sheet1!$13:$13,Sheet1!$14:$14,Sheet1!$15:$15</definedName>
     <definedName name="QB_DATE_1" localSheetId="1" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="QB_FORMULA_0" localSheetId="1" hidden="1">Sheet1!$C$35,Sheet1!$E$35</definedName>
-    <definedName name="QB_ROW_101210" localSheetId="1" hidden="1">Sheet1!$B$26</definedName>
-    <definedName name="QB_ROW_102210" localSheetId="1" hidden="1">Sheet1!$B$27</definedName>
-    <definedName name="QB_ROW_107210" localSheetId="1" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="QB_ROW_111210" localSheetId="1" hidden="1">Sheet1!$B$29</definedName>
-    <definedName name="QB_ROW_115210" localSheetId="1" hidden="1">Sheet1!$B$30</definedName>
-    <definedName name="QB_ROW_121210" localSheetId="1" hidden="1">Sheet1!$B$31</definedName>
-    <definedName name="QB_ROW_14210" localSheetId="1" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="QB_ROW_154210" localSheetId="1" hidden="1">Sheet1!$B$32</definedName>
-    <definedName name="QB_ROW_168210" localSheetId="1" hidden="1">Sheet1!$B$34</definedName>
-    <definedName name="QB_ROW_174210" localSheetId="1" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="QB_ROW_175210" localSheetId="1" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="QB_ROW_176210" localSheetId="1" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="QB_ROW_177210" localSheetId="1" hidden="1">Sheet1!$B$22</definedName>
-    <definedName name="QB_ROW_178210" localSheetId="1" hidden="1">Sheet1!$B$33</definedName>
-    <definedName name="QB_ROW_18210" localSheetId="1" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="QB_ROW_25301" localSheetId="1" hidden="1">Sheet1!$A$35</definedName>
-    <definedName name="QB_ROW_41210" localSheetId="1" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="QB_ROW_43210" localSheetId="1" hidden="1">Sheet1!$B$10</definedName>
-    <definedName name="QB_ROW_44210" localSheetId="1" hidden="1">Sheet1!$B$11</definedName>
-    <definedName name="QB_ROW_66210" localSheetId="1" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="QB_ROW_69210" localSheetId="1" hidden="1">Sheet1!$B$13</definedName>
-    <definedName name="QB_ROW_70210" localSheetId="1" hidden="1">Sheet1!$B$14</definedName>
-    <definedName name="QB_ROW_74210" localSheetId="1" hidden="1">Sheet1!$B$15</definedName>
-    <definedName name="QB_ROW_76210" localSheetId="1" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="QB_ROW_80210" localSheetId="1" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="QB_ROW_81210" localSheetId="1" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="QB_ROW_86210" localSheetId="1" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="QB_ROW_87210" localSheetId="1" hidden="1">Sheet1!$B$23</definedName>
-    <definedName name="QB_ROW_88210" localSheetId="1" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="QB_ROW_89210" localSheetId="1" hidden="1">Sheet1!$B$25</definedName>
+    <definedName name="QB_FORMULA_0" localSheetId="1" hidden="1">Sheet1!$C$16,Sheet1!$E$16</definedName>
+    <definedName name="QB_ROW_13210" localSheetId="1" hidden="1">Sheet1!$B$7</definedName>
+    <definedName name="QB_ROW_141210" localSheetId="1" hidden="1">Sheet1!$B$10</definedName>
+    <definedName name="QB_ROW_153210" localSheetId="1" hidden="1">Sheet1!$B$11</definedName>
+    <definedName name="QB_ROW_154210" localSheetId="1" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="QB_ROW_175210" localSheetId="1" hidden="1">Sheet1!$B$13</definedName>
+    <definedName name="QB_ROW_192210" localSheetId="1" hidden="1">Sheet1!$B$6</definedName>
+    <definedName name="QB_ROW_193210" localSheetId="1" hidden="1">Sheet1!$B$15</definedName>
+    <definedName name="QB_ROW_194210" localSheetId="1" hidden="1">Sheet1!$B$8</definedName>
+    <definedName name="QB_ROW_195210" localSheetId="1" hidden="1">Sheet1!$B$14</definedName>
+    <definedName name="QB_ROW_25301" localSheetId="1" hidden="1">Sheet1!$A$16</definedName>
+    <definedName name="QB_ROW_27210" localSheetId="1" hidden="1">Sheet1!$B$9</definedName>
     <definedName name="QB_SUBTITLE_3" localSheetId="1" hidden="1">Sheet1!$A$3</definedName>
     <definedName name="QB_TIME_5" localSheetId="1" hidden="1">Sheet1!$E$1</definedName>
     <definedName name="QB_TITLE_2" localSheetId="1" hidden="1">Sheet1!$A$2</definedName>
     <definedName name="QBCANSUPPORTUPDATE" localSheetId="1">TRUE</definedName>
-    <definedName name="QBCOMPANYFILENAME" localSheetId="1">"\\data23\home23$\saltmarsh5\Desktop\Access Client QB\Tampa Squad\EPG\2022 QB Backups\PBC\EPG West Hillcrest Holdings\EPG West Hillcrest Holdings, LLC.QBW"</definedName>
+    <definedName name="QBCOMPANYFILENAME" localSheetId="1">"\\data23\home23$\saltmarsh5\Desktop\Access Client QB\Tampa Squad\EPG\2022 QB Backups\PBC\EPG Two Rivers QOF 2022\EPG Two Rivers QOF 2022, LLC.QBW"</definedName>
     <definedName name="QBENDDATE" localSheetId="1">20221231</definedName>
     <definedName name="QBHEADERSONSCREEN" localSheetId="1">TRUE</definedName>
     <definedName name="QBMETADATASIZE" localSheetId="1">5924</definedName>
@@ -71,7 +51,7 @@
     <definedName name="QBPRESERVEROWHEIGHT" localSheetId="1">TRUE</definedName>
     <definedName name="QBPRESERVESPACE" localSheetId="1">TRUE</definedName>
     <definedName name="QBREPORTCOLAXIS" localSheetId="1">0</definedName>
-    <definedName name="QBREPORTCOMPANYID" localSheetId="1">"5a8de130f8ab4919acba16cb0bd80941"</definedName>
+    <definedName name="QBREPORTCOMPANYID" localSheetId="1">"cdb5aed093ca4875bac2f053f10a5419"</definedName>
     <definedName name="QBREPORTCOMPARECOL_ANNUALBUDGET" localSheetId="1">FALSE</definedName>
     <definedName name="QBREPORTCOMPARECOL_AVGCOGS" localSheetId="1">FALSE</definedName>
     <definedName name="QBREPORTCOMPARECOL_AVGPRICE" localSheetId="1">FALSE</definedName>
@@ -134,9 +114,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>8:13 PM</t>
+    <t>8:03 PM</t>
   </si>
   <si>
     <t>Trial Balance</t>
@@ -157,64 +137,10 @@
     <t>Credit</t>
   </si>
   <si>
-    <t>13010 · Land Held for Investment:13011 · Land Basis:13011.1 · Land</t>
+    <t>1250 · Accounts Receivable</t>
   </si>
   <si>
-    <t>13010 · Land Held for Investment:13011 · Land Basis:13011.3 · Assignment Fee</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:13011 · Land Basis:13012 · Closing Cost</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:13011 · Land Basis:13013 · Property Taxes</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:13060 · Financing Cost:13061 · Interest</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:13060 · Financing Cost:13064 · Closing Cost</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:13060 · Financing Cost:13065 · Origination Fee</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:13022 · Property Insurance</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14002 · Surveying</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14006 · Government fees</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14007 · Ecological</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14012 · Admin. Costs</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14013 · Consultants</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14014 · Engineering</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14015 · Environmental</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14021 · Legal</t>
-  </si>
-  <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14022 · Closing Costs</t>
-  </si>
-  <si>
-    <t>20000 · Accounts Payable</t>
-  </si>
-  <si>
-    <t>20000.1 · UNAPPROVED A/P</t>
-  </si>
-  <si>
-    <t>2333 · Accrued Interest Payable</t>
+    <t>12000 · Undeposited Funds</t>
   </si>
   <si>
     <t>60400 · Bank Service Charges</t>
@@ -223,31 +149,28 @@
     <t>67300 · Management Fee Exp.</t>
   </si>
   <si>
-    <t>69000 · Political Contribution</t>
+    <t>70000 · Interest Income</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>ABC Subsidiary, LLC</t>
+    <t>DEF Subsidiary, LLC</t>
   </si>
   <si>
-    <t>1010 · Example Bank - Business Banking</t>
+    <t xml:space="preserve">1010 · Example Bank - Business Banking </t>
   </si>
   <si>
-    <t>1210 · Cash In Transit</t>
+    <t>1261 · Loan Receivable - ABC</t>
   </si>
   <si>
-    <t>13010 · Land Held for Investment:14000 · Other Costs:14098 · Cap. Costs from DEF</t>
+    <t>20100 · Due To/(From) Related Entities:20102 · Due To/(From) - FGH</t>
   </si>
   <si>
-    <t>20100 · Due To/(From) Related Entities:20101 · Due To/(From) - YZ Subsidiary</t>
+    <t>30300 · Capital Account - Jeff:30301 · Capital Account - Jane Doe</t>
   </si>
   <si>
-    <t>20050 · Home Builder Deposits:20051 · Contractor X, LLC</t>
-  </si>
-  <si>
-    <t>20400 · Notes Payable:20401 · Note Payable - John Doe</t>
+    <t>30300 · Capital Account - Jeff:30302 · Member Draw - Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -375,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -421,8 +344,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="40" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1726,28 +1647,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="9" customWidth="1"/>
-    <col min="2" max="2" width="86.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -1756,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1687,7 @@
         <v>44987</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -1778,7 +1698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
@@ -1787,7 +1707,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="18" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="18" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16" t="s">
@@ -1798,366 +1718,132 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6">
-        <v>716.8</v>
+        <v>700</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
-      <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
-      <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6">
-        <v>3561613.12</v>
+        <v>0</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
-      <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C9" s="6">
-        <v>131260</v>
+        <v>10000000</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
-      <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6">
-        <v>48155.45</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="G10" s="21"/>
+      <c r="E10" s="6">
+        <v>30000</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6">
-        <v>537.41999999999996</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="6">
+        <v>10000000</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C12" s="6">
-        <v>245590.42</v>
+        <v>100000</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6"/>
-      <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6">
-        <v>14600</v>
+        <v>200</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="6"/>
-      <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6">
-        <v>39700</v>
+        <v>30000</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
-      <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1252.95</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="6"/>
-      <c r="G15" s="21"/>
+      <c r="E15" s="6">
+        <v>100900</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6">
-        <v>419508.7</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
-      <c r="G16" s="21"/>
+    <row r="16" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="8">
+        <f>ROUND(SUM(C6:C15),5)</f>
+        <v>10130900</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="8">
+        <f>ROUND(SUM(E6:E15),5)</f>
+        <v>10130900</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="6">
-        <v>63262</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="6">
-        <v>6800</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
-      <c r="G18" s="21"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6">
-        <v>14701.99</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="6">
-        <v>8262.5</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="6">
-        <v>23560.799999999999</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="6">
-        <v>55140.24</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="6">
-        <v>42555.73</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="6">
-        <v>28575.75</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="6">
-        <v>113822.81</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6">
-        <v>66992.31</v>
-      </c>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6">
-        <v>103956</v>
-      </c>
-      <c r="G27" s="21"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6">
-        <v>4683500</v>
-      </c>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6">
-        <v>24945.21</v>
-      </c>
-      <c r="G29" s="21"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="6">
-        <v>1043861.84</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="6">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="6">
-        <v>515</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="6">
-        <v>15400</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="6">
-        <v>0</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="8">
-        <f>ROUND(SUM(C6:C34),5)</f>
-        <v>5879393.5199999996</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="8">
-        <f>ROUND(SUM(E6:E34),5)</f>
-        <v>5879393.5199999996</v>
-      </c>
-      <c r="G35" s="22"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.1" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>